<commit_message>
Remove show more/show less toggle from issuer bio - always display full bio
</commit_message>
<xml_diff>
--- a/pauvfeb.xlsx
+++ b/pauvfeb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daven\Desktop\pauvfeb2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6913DC04-C056-453C-95E8-CBA83719FFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79F8FB6-B248-4A81-AB93-F7B141A4B0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{5E8491D6-7D25-4ABD-8652-15E2B468F991}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12456" xr2:uid="{5E8491D6-7D25-4ABD-8652-15E2B468F991}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,9 +43,6 @@
   </si>
   <si>
     <t>Email sign in</t>
-  </si>
-  <si>
-    <t>Stripe connection</t>
   </si>
   <si>
     <t>Top Site</t>
@@ -333,6 +329,9 @@
   <si>
     <t>avg_cost_basis</t>
   </si>
+  <si>
+    <t>Soap connection</t>
+  </si>
 </sst>
 </file>
 
@@ -342,8 +341,8 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="182" formatCode="_(* #,##0.00000000000000_);_(* \(#,##0.00000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000000000000_);_(* \(#,##0.00000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -433,10 +432,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -450,10 +448,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -773,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9650B0-1321-479B-B743-1617EA350E0C}">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -787,7 +785,7 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -802,116 +800,116 @@
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="C21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="C25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="C26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -935,58 +933,58 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1016,104 +1014,104 @@
   <sheetData>
     <row r="2" spans="1:3" ht="15" thickBot="1"/>
     <row r="3" spans="1:3" ht="15" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="28.5" thickBot="1">
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.5" thickBot="1">
-      <c r="A4" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" thickBot="1">
+      <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5" thickBot="1">
+      <c r="A6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5" thickBot="1">
+      <c r="A7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29" thickBot="1">
+      <c r="A8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1">
+      <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.5" thickBot="1">
-      <c r="A5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" thickBot="1">
-      <c r="A6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" thickBot="1">
-      <c r="A7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29" thickBot="1">
-      <c r="A8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="28.5" thickBot="1">
+      <c r="A10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5" thickBot="1">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="6">
+        <v>42</v>
+      </c>
+      <c r="B14" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15">
         <v>0.01</v>
@@ -1121,127 +1119,127 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
         <v>54</v>
       </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
       <c r="F17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
         <v>77</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>81</v>
       </c>
-      <c r="H22" t="s">
-        <v>80</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>82</v>
-      </c>
-      <c r="J22" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
-        <v>79</v>
-      </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
         <v>86</v>
-      </c>
-      <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDAB284-8C0D-43AF-8DE1-802E90F55DC2}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1268,7 +1266,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1">
         <v>0.01</v>
@@ -1276,7 +1274,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
@@ -1284,111 +1282,111 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>69</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>100</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <f>(-B1+SQRT(B1^2+2*B2*A4))/B2</f>
         <v>437.32538492690082</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f>B1 + (D4 * B2)</f>
         <v>0.44732538492690083</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>B4</f>
         <v>437.32538492690082</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <f>A4</f>
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>5</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <f>(-C4+SQRT(C4^2+2*$B$2*A5))/$B$2</f>
         <v>11.041280527732788</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <f>B$1+(D5*B$2)</f>
         <v>0.45836666545463361</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f>D4+B5</f>
         <v>448.36666545463362</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <f>E4+A5</f>
         <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <f>(-C5+SQRT(C5^2+2*$B$2*A6))/$B$2</f>
         <v>10.781498774962428</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f>B$1+(D6*B$2)</f>
         <v>0.46914816422959604</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <f>D5+B6</f>
         <v>459.14816422959603</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <f>E5+A6</f>
         <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>(-C6+SQRT(C6^2+2*$B$2*A7))/$B$2</f>
         <v>10.539233978862249</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <f>B$1+(D7*B$2)</f>
         <v>0.47968739820845829</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <f>D6+B7</f>
         <v>469.68739820845826</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <f>E6+A7</f>
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8" s="8"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="8"/>
-      <c r="C9" s="12">
+      <c r="B9" s="7"/>
+      <c r="C9" s="11">
         <f>C7/B1</f>
         <v>47.968739820845826</v>
       </c>

</xml_diff>